<commit_message>
Lots of small text changes
</commit_message>
<xml_diff>
--- a/frontend/src/assets/Excel_Import.xlsx
+++ b/frontend/src/assets/Excel_Import.xlsx
@@ -213,9 +213,6 @@
     <t>Maatwerk project eigenschappen</t>
   </si>
   <si>
-    <t>Waarde categorie</t>
-  </si>
-  <si>
     <t>Huurprijs categorie</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>Woningblok 8</t>
+  </si>
+  <si>
+    <t>Koopprijs categorie</t>
   </si>
 </sst>
 </file>
@@ -1017,16 +1017,16 @@
         <v>27</v>
       </c>
       <c r="L4" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="N4" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="O4" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1401,7 +1401,7 @@
         <v>23</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -1418,7 +1418,7 @@
       <c r="D30" s="34"/>
       <c r="F30" s="25"/>
       <c r="G30" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="33" spans="2:15">
       <c r="F33" s="23" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="G33" s="39"/>
       <c r="H33" s="34"/>
@@ -1588,7 +1588,7 @@
       <c r="C40" s="35"/>
       <c r="D40" s="34"/>
       <c r="F40" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G40" s="39"/>
       <c r="H40" s="34"/>
@@ -1720,7 +1720,7 @@
         <v>22</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H48" s="34"/>
       <c r="I48" s="34"/>
@@ -1739,7 +1739,7 @@
       <c r="D49" s="34"/>
       <c r="F49" s="26"/>
       <c r="G49" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
@@ -1777,7 +1777,7 @@
         <v>63</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H51" s="34"/>
       <c r="I51" s="34"/>
@@ -1796,7 +1796,7 @@
       <c r="D52" s="34"/>
       <c r="F52" s="25"/>
       <c r="G52" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
@@ -1810,7 +1810,7 @@
     <row r="53" spans="2:15">
       <c r="F53" s="25"/>
       <c r="G53" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H53" s="34"/>
       <c r="I53" s="34"/>
@@ -1829,7 +1829,7 @@
       <c r="D54" s="8"/>
       <c r="F54" s="25"/>
       <c r="G54" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H55" s="34"/>
       <c r="I55" s="34"/>
@@ -1869,7 +1869,7 @@
       <c r="D56" s="34"/>
       <c r="F56" s="26"/>
       <c r="G56" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
@@ -1910,7 +1910,7 @@
         <v>33</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H59" s="34"/>
       <c r="I59" s="34"/>
@@ -1927,7 +1927,7 @@
       <c r="D60" s="34"/>
       <c r="F60" s="25"/>
       <c r="G60" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
@@ -1944,7 +1944,7 @@
       <c r="D61" s="34"/>
       <c r="F61" s="25"/>
       <c r="G61" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H61" s="34"/>
       <c r="I61" s="34"/>
@@ -1961,7 +1961,7 @@
       <c r="D62" s="34"/>
       <c r="F62" s="25"/>
       <c r="G62" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H62" s="34"/>
       <c r="I62" s="34"/>
@@ -1978,7 +1978,7 @@
       <c r="D63" s="34"/>
       <c r="F63" s="25"/>
       <c r="G63" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="34"/>
@@ -1995,7 +1995,7 @@
       <c r="D64" s="34"/>
       <c r="F64" s="26"/>
       <c r="G64" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="72" spans="2:15">
       <c r="F72" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="34"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="73" spans="2:15">
       <c r="F73" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G73" s="20"/>
       <c r="H73" s="34"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="74" spans="2:15">
       <c r="F74" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G74" s="20"/>
       <c r="H74" s="34"/>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="76" spans="2:15">
       <c r="F76" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G76" s="30"/>
       <c r="H76" s="22"/>

</xml_diff>